<commit_message>
Raw data was processed by aligning each PEER scan to the first of each participant. SVR model works well for several participants, while others have predicted values that exceed the range of expected values (e.g. 1-2 orders of magnitude). Currently testing with different methods of preprocessing (w/ or w/o motion correction, different possible C and epsilon values).
</commit_message>
<xml_diff>
--- a/subj_params.xlsx
+++ b/subj_params.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1540" yWindow="3960" windowWidth="10000" windowHeight="16860" tabRatio="500"/>
+    <workbookView xWindow="2140" yWindow="3240" windowWidth="13820" windowHeight="16860" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>Subject</t>
   </si>
@@ -57,6 +57,39 @@
   </si>
   <si>
     <t>c</t>
+  </si>
+  <si>
+    <t>one</t>
+  </si>
+  <si>
+    <t>three</t>
+  </si>
+  <si>
+    <t>four</t>
+  </si>
+  <si>
+    <t>five</t>
+  </si>
+  <si>
+    <t>v3_c</t>
+  </si>
+  <si>
+    <t>v3_d</t>
+  </si>
+  <si>
+    <t>v3_e</t>
+  </si>
+  <si>
+    <t>v3_a</t>
+  </si>
+  <si>
+    <t>Reason</t>
+  </si>
+  <si>
+    <t>Magnitude (x)</t>
+  </si>
+  <si>
+    <t>Magnitude (x,y)</t>
   </si>
 </sst>
 </file>
@@ -72,12 +105,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -92,8 +143,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -371,15 +425,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="8" max="8" width="14.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -401,9 +458,12 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="H1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B2">
@@ -425,8 +485,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B3">
@@ -447,9 +507,12 @@
       <c r="G3">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="H3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B4">
@@ -469,6 +532,202 @@
       </c>
       <c r="G4">
         <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>14</v>
+      </c>
+      <c r="C5">
+        <v>39</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>12</v>
+      </c>
+      <c r="F5">
+        <v>9</v>
+      </c>
+      <c r="G5">
+        <v>18</v>
+      </c>
+      <c r="H5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>14</v>
+      </c>
+      <c r="C6">
+        <v>39</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6">
+        <v>13</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7">
+        <v>14</v>
+      </c>
+      <c r="C7">
+        <v>39</v>
+      </c>
+      <c r="D7">
+        <v>7</v>
+      </c>
+      <c r="E7">
+        <v>17</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>9</v>
+      </c>
+      <c r="H7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>13</v>
+      </c>
+      <c r="C8">
+        <v>39</v>
+      </c>
+      <c r="D8">
+        <v>8</v>
+      </c>
+      <c r="E8">
+        <v>17</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8">
+        <v>10</v>
+      </c>
+      <c r="H8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9">
+        <v>14</v>
+      </c>
+      <c r="C9">
+        <v>40</v>
+      </c>
+      <c r="D9">
+        <v>3</v>
+      </c>
+      <c r="E9">
+        <v>11</v>
+      </c>
+      <c r="F9">
+        <v>8</v>
+      </c>
+      <c r="G9">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10">
+        <v>14</v>
+      </c>
+      <c r="C10">
+        <v>40</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="E10">
+        <v>12</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11">
+        <v>17</v>
+      </c>
+      <c r="C11">
+        <v>38</v>
+      </c>
+      <c r="D11">
+        <v>8</v>
+      </c>
+      <c r="E11">
+        <v>18</v>
+      </c>
+      <c r="F11">
+        <v>3</v>
+      </c>
+      <c r="G11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12">
+        <v>18</v>
+      </c>
+      <c r="C12">
+        <v>40</v>
+      </c>
+      <c r="D12">
+        <v>8</v>
+      </c>
+      <c r="E12">
+        <v>16</v>
+      </c>
+      <c r="F12">
+        <v>3</v>
+      </c>
+      <c r="G12">
+        <v>10</v>
+      </c>
+      <c r="H12" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Compared outputs for motion corrected data and raw data (both registered to first PEER scan of each participant). For now, motion correction will not be used since there is no demonstrable benefit (may change upon further analysis).
</commit_message>
<xml_diff>
--- a/subj_params.xlsx
+++ b/subj_params.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2140" yWindow="3240" windowWidth="13820" windowHeight="16860" tabRatio="500"/>
+    <workbookView xWindow="8980" yWindow="3200" windowWidth="13820" windowHeight="16860" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>Subject</t>
   </si>
@@ -50,46 +50,37 @@
     <t>z_end</t>
   </si>
   <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>one</t>
-  </si>
-  <si>
-    <t>three</t>
-  </si>
-  <si>
-    <t>four</t>
-  </si>
-  <si>
-    <t>five</t>
-  </si>
-  <si>
-    <t>v3_c</t>
-  </si>
-  <si>
-    <t>v3_d</t>
-  </si>
-  <si>
-    <t>v3_e</t>
-  </si>
-  <si>
-    <t>v3_a</t>
-  </si>
-  <si>
     <t>Reason</t>
   </si>
   <si>
-    <t>Magnitude (x)</t>
-  </si>
-  <si>
     <t>Magnitude (x,y)</t>
+  </si>
+  <si>
+    <t>n5548204</t>
+  </si>
+  <si>
+    <t>n5614104</t>
+  </si>
+  <si>
+    <t>n5668069</t>
+  </si>
+  <si>
+    <t>n5106395</t>
+  </si>
+  <si>
+    <t>n5075903</t>
+  </si>
+  <si>
+    <t>n5026599</t>
+  </si>
+  <si>
+    <t>n5000946</t>
+  </si>
+  <si>
+    <t>5075903_mc</t>
+  </si>
+  <si>
+    <t>5106395_mc</t>
   </si>
 </sst>
 </file>
@@ -425,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="A11" sqref="A11:A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -459,278 +450,226 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="B2">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2">
         <v>40</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E2">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F2">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G2">
         <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>8</v>
+      <c r="A3" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="B3">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D3">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E3">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G3">
-        <v>8</v>
-      </c>
-      <c r="H3" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B4">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C4">
         <v>38</v>
       </c>
       <c r="D4">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E4">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="F4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G4">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5">
+        <v>18</v>
+      </c>
+      <c r="C5">
+        <v>40</v>
+      </c>
+      <c r="D5">
+        <v>8</v>
+      </c>
+      <c r="E5">
+        <v>16</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5">
         <v>10</v>
       </c>
-      <c r="B5">
-        <v>14</v>
-      </c>
-      <c r="C5">
-        <v>39</v>
-      </c>
-      <c r="D5">
-        <v>2</v>
-      </c>
-      <c r="E5">
-        <v>12</v>
-      </c>
-      <c r="F5">
+      <c r="H5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G5">
+      <c r="B6">
+        <v>16</v>
+      </c>
+      <c r="C6">
+        <v>35</v>
+      </c>
+      <c r="D6">
+        <v>8</v>
+      </c>
+      <c r="E6">
         <v>18</v>
       </c>
-      <c r="H5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6">
-        <v>14</v>
-      </c>
-      <c r="C6">
-        <v>39</v>
-      </c>
-      <c r="D6">
-        <v>3</v>
-      </c>
-      <c r="E6">
-        <v>13</v>
-      </c>
       <c r="F6">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G6">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B7">
+        <v>16</v>
+      </c>
+      <c r="C7">
+        <v>40</v>
+      </c>
+      <c r="D7">
+        <v>4</v>
+      </c>
+      <c r="E7">
+        <v>16</v>
+      </c>
+      <c r="F7">
+        <v>3</v>
+      </c>
+      <c r="G7">
+        <v>11</v>
+      </c>
+      <c r="H7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>16</v>
+      </c>
+      <c r="C8">
+        <v>40</v>
+      </c>
+      <c r="D8">
+        <v>4</v>
+      </c>
+      <c r="E8">
         <v>14</v>
       </c>
-      <c r="C7">
-        <v>39</v>
-      </c>
-      <c r="D7">
-        <v>7</v>
-      </c>
-      <c r="E7">
+      <c r="F8">
+        <v>3</v>
+      </c>
+      <c r="G8">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9">
         <v>17</v>
       </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7">
-        <v>9</v>
-      </c>
-      <c r="H7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8">
-        <v>13</v>
-      </c>
-      <c r="C8">
-        <v>39</v>
-      </c>
-      <c r="D8">
-        <v>8</v>
-      </c>
-      <c r="E8">
+      <c r="C9">
+        <v>38</v>
+      </c>
+      <c r="D9">
+        <v>8</v>
+      </c>
+      <c r="E9">
+        <v>18</v>
+      </c>
+      <c r="F9">
+        <v>3</v>
+      </c>
+      <c r="G9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>17</v>
       </c>
-      <c r="F8">
-        <v>2</v>
-      </c>
-      <c r="G8">
-        <v>10</v>
-      </c>
-      <c r="H8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9">
-        <v>14</v>
-      </c>
-      <c r="C9">
-        <v>40</v>
-      </c>
-      <c r="D9">
-        <v>3</v>
-      </c>
-      <c r="E9">
-        <v>11</v>
-      </c>
-      <c r="F9">
-        <v>8</v>
-      </c>
-      <c r="G9">
+      <c r="B10">
         <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10">
-        <v>14</v>
       </c>
       <c r="C10">
         <v>40</v>
       </c>
       <c r="D10">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E10">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="F10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G10">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11">
-        <v>17</v>
-      </c>
-      <c r="C11">
-        <v>38</v>
-      </c>
-      <c r="D11">
-        <v>8</v>
-      </c>
-      <c r="E11">
-        <v>18</v>
-      </c>
-      <c r="F11">
-        <v>3</v>
-      </c>
-      <c r="G11">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12">
-        <v>18</v>
-      </c>
-      <c r="C12">
-        <v>40</v>
-      </c>
-      <c r="D12">
-        <v>8</v>
-      </c>
-      <c r="E12">
-        <v>16</v>
-      </c>
-      <c r="F12">
-        <v>3</v>
-      </c>
-      <c r="G12">
-        <v>10</v>
-      </c>
-      <c r="H12" t="s">
-        <v>20</v>
-      </c>
-    </row>
   </sheetData>
+  <sortState ref="A2:H8">
+    <sortCondition ref="A1"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Figures saved to separat outpath. Milestones/issues to be updated.
</commit_message>
<xml_diff>
--- a/subj_params.xlsx
+++ b/subj_params.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8980" yWindow="3200" windowWidth="13820" windowHeight="16860" tabRatio="500"/>
+    <workbookView xWindow="11600" yWindow="1020" windowWidth="13820" windowHeight="16860" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
   <si>
     <t>Subject</t>
   </si>
@@ -81,6 +81,33 @@
   </si>
   <si>
     <t>5106395_mc</t>
+  </si>
+  <si>
+    <t>n5072755</t>
+  </si>
+  <si>
+    <t>n5178472</t>
+  </si>
+  <si>
+    <t>Low MFD</t>
+  </si>
+  <si>
+    <t>High MFD</t>
+  </si>
+  <si>
+    <t>n5979692</t>
+  </si>
+  <si>
+    <t>n5518313</t>
+  </si>
+  <si>
+    <t>n5910480</t>
+  </si>
+  <si>
+    <t>Data Quality</t>
+  </si>
+  <si>
+    <t>n5773707</t>
   </si>
 </sst>
 </file>
@@ -134,11 +161,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -416,18 +444,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:A13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="8" max="8" width="14.83203125" customWidth="1"/>
+    <col min="9" max="9" width="12.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -452,8 +481,11 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -476,7 +508,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -499,7 +531,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
@@ -522,7 +554,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
@@ -548,7 +580,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -571,7 +603,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
@@ -597,7 +629,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -620,8 +652,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B9">
@@ -642,9 +674,12 @@
       <c r="G9">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="H9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B10">
@@ -665,6 +700,219 @@
       <c r="G10">
         <v>10</v>
       </c>
+      <c r="H10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11">
+        <v>14</v>
+      </c>
+      <c r="C11">
+        <v>40</v>
+      </c>
+      <c r="D11">
+        <v>35</v>
+      </c>
+      <c r="E11">
+        <v>45</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>10</v>
+      </c>
+      <c r="I11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12">
+        <v>12</v>
+      </c>
+      <c r="C12">
+        <v>38</v>
+      </c>
+      <c r="D12">
+        <v>38</v>
+      </c>
+      <c r="E12">
+        <v>48</v>
+      </c>
+      <c r="F12">
+        <v>4</v>
+      </c>
+      <c r="G12">
+        <v>12</v>
+      </c>
+      <c r="I12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13">
+        <v>14</v>
+      </c>
+      <c r="C13">
+        <v>40</v>
+      </c>
+      <c r="D13">
+        <v>37</v>
+      </c>
+      <c r="E13">
+        <v>45</v>
+      </c>
+      <c r="F13">
+        <v>4</v>
+      </c>
+      <c r="G13">
+        <v>12</v>
+      </c>
+      <c r="I13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14">
+        <v>14</v>
+      </c>
+      <c r="C14">
+        <v>40</v>
+      </c>
+      <c r="D14">
+        <v>37</v>
+      </c>
+      <c r="E14">
+        <v>46</v>
+      </c>
+      <c r="F14">
+        <v>5</v>
+      </c>
+      <c r="G14">
+        <v>13</v>
+      </c>
+      <c r="I14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15">
+        <v>13</v>
+      </c>
+      <c r="C15">
+        <v>36</v>
+      </c>
+      <c r="D15">
+        <v>38</v>
+      </c>
+      <c r="E15">
+        <v>47</v>
+      </c>
+      <c r="F15">
+        <v>2</v>
+      </c>
+      <c r="G15">
+        <v>11</v>
+      </c>
+      <c r="I15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16">
+        <v>38</v>
+      </c>
+      <c r="D16">
+        <v>39</v>
+      </c>
+      <c r="E16">
+        <v>46</v>
+      </c>
+      <c r="F16">
+        <v>3</v>
+      </c>
+      <c r="G16">
+        <v>10</v>
+      </c>
+      <c r="I16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="4"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="4"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="4"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="4"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" s="4"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" s="4"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" s="4"/>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" s="4"/>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" s="4"/>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" s="4"/>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" s="4"/>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" s="4"/>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" s="4"/>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" s="4"/>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" s="4"/>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" s="4"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" s="4"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" s="4"/>
     </row>
   </sheetData>
   <sortState ref="A2:H8">

</xml_diff>